<commit_message>
new plots and pdf
</commit_message>
<xml_diff>
--- a/CHORUS.xlsx
+++ b/CHORUS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,17 +24,20 @@
     <definedName function="false" hidden="false" name="PropsedYr3" vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="Print_Area_0" vbProcedure="false">'Anticipated non-NCE Funding'!$A$1:$G$17</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'Anticipated non-NCE Funding'!$A$1:$G$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0" vbProcedure="false">'Anticipated non-NCE Funding'!$A$1:$G$17</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Print_Area_0" vbProcedure="false">'Partners '!$A$1:$I$103</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Print_Titles_0" vbProcedure="false">'Partners '!$4:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Partners '!$A$1:$I$103</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0" vbProcedure="false">'Partners '!$A$1:$I$103</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Titles" vbProcedure="false">'Partners '!$4:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Titles_0" vbProcedure="false">'Partners '!$4:$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="147">
   <si>
     <t>Instructions</t>
   </si>
@@ -483,22 +486,19 @@
     <t>NS</t>
   </si>
   <si>
-    <t>ESA</t>
-  </si>
-  <si>
-    <t>Arviset</t>
-  </si>
-  <si>
-    <t>Christophe</t>
-  </si>
-  <si>
-    <t>Data and Engineering Division</t>
+    <t>HIA</t>
+  </si>
+  <si>
+    <t>Schade</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>CADC</t>
   </si>
   <si>
     <t>Head</t>
-  </si>
-  <si>
-    <t>Spain</t>
   </si>
   <si>
     <t>Interoperability</t>
@@ -1630,7 +1630,7 @@
   </sheetPr>
   <dimension ref="1:22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -4752,8 +4752,8 @@
   </sheetPr>
   <dimension ref="A1:AB103"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -5145,16 +5145,16 @@
         <v>123</v>
       </c>
       <c r="G14" s="90" t="s">
-        <v>124</v>
+        <v>62</v>
       </c>
       <c r="H14" s="90" t="n">
         <v>5</v>
       </c>
       <c r="I14" s="93" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB14" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="AB14" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5172,7 +5172,7 @@
       <c r="H15" s="92"/>
       <c r="I15" s="92"/>
       <c r="AB15" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5186,7 +5186,7 @@
       <c r="H16" s="90"/>
       <c r="I16" s="93"/>
       <c r="AB16" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5200,7 +5200,7 @@
       <c r="H17" s="95"/>
       <c r="I17" s="97"/>
       <c r="AB17" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5214,7 +5214,7 @@
       <c r="H18" s="90"/>
       <c r="I18" s="93"/>
       <c r="AB18" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6200,11 +6200,11 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="84" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B2" s="84"/>
       <c r="C2" s="100" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D2" s="83"/>
       <c r="E2" s="84"/>
@@ -6214,7 +6214,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="82"/>
@@ -6226,31 +6226,31 @@
     </row>
     <row r="4" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="101" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" s="101"/>
       <c r="C4" s="102" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="102" t="s">
         <v>135</v>
       </c>
-      <c r="D4" s="102" t="s">
+      <c r="E4" s="102" t="s">
         <v>136</v>
       </c>
-      <c r="E4" s="102" t="s">
+      <c r="F4" s="102" t="s">
         <v>137</v>
       </c>
-      <c r="F4" s="102" t="s">
+      <c r="G4" s="102" t="s">
         <v>138</v>
       </c>
-      <c r="G4" s="102" t="s">
+      <c r="H4" s="103" t="s">
         <v>139</v>
-      </c>
-      <c r="H4" s="103" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="104" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5" s="104"/>
       <c r="C5" s="105"/>
@@ -6265,7 +6265,7 @@
     </row>
     <row r="6" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="104" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B6" s="104"/>
       <c r="C6" s="105"/>
@@ -6280,7 +6280,7 @@
     </row>
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="104" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" s="104"/>
       <c r="C7" s="105"/>
@@ -6295,7 +6295,7 @@
     </row>
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="104" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B8" s="104"/>
       <c r="C8" s="105"/>
@@ -6311,7 +6311,7 @@
     </row>
     <row r="9" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="104" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B9" s="104"/>
       <c r="C9" s="105"/>
@@ -6326,7 +6326,7 @@
     </row>
     <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="109" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B10" s="110"/>
       <c r="C10" s="105"/>
@@ -6341,7 +6341,7 @@
     </row>
     <row r="11" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="111" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B11" s="111"/>
       <c r="C11" s="112"/>

</xml_diff>